<commit_message>
date and webelement utlity
</commit_message>
<xml_diff>
--- a/Qa_Legend/src/main/resources/TestData.xlsx
+++ b/Qa_Legend/src/main/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13815" windowHeight="3060" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13815" windowHeight="3060"/>
   </bookViews>
   <sheets>
     <sheet name="Home_Page" sheetId="3" r:id="rId1"/>
@@ -14,7 +14,6 @@
     <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N8"/>
 </workbook>
 </file>
 
@@ -419,7 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -450,7 +449,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>